<commit_message>
Enhance order management: update SQL queries for discounts, refactor order item retrieval, and improve UI for displaying product details
</commit_message>
<xml_diff>
--- a/Backup/Discounts.xlsx
+++ b/Backup/Discounts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1226,6 +1226,330 @@
         <v>0</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2</v>
+      </c>
+      <c r="C30" t="n">
+        <v>31</v>
+      </c>
+      <c r="D30" t="n">
+        <v>10</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-03-03 17:38:18</t>
+        </is>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2</v>
+      </c>
+      <c r="C31" t="n">
+        <v>32</v>
+      </c>
+      <c r="D31" t="n">
+        <v>6</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-03-03 17:44:09</t>
+        </is>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2</v>
+      </c>
+      <c r="C32" t="n">
+        <v>33</v>
+      </c>
+      <c r="D32" t="n">
+        <v>20</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-03-03 17:45:14</t>
+        </is>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" t="n">
+        <v>34</v>
+      </c>
+      <c r="D33" t="n">
+        <v>20</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-03-03 17:45:56</t>
+        </is>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2</v>
+      </c>
+      <c r="C34" t="n">
+        <v>35</v>
+      </c>
+      <c r="D34" t="n">
+        <v>4</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-03-03 17:49:17</t>
+        </is>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2</v>
+      </c>
+      <c r="C35" t="n">
+        <v>36</v>
+      </c>
+      <c r="D35" t="n">
+        <v>3</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>2025-03-03 17:50:02</t>
+        </is>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2</v>
+      </c>
+      <c r="C36" t="n">
+        <v>37</v>
+      </c>
+      <c r="D36" t="n">
+        <v>3</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>2025-03-03 17:53:52</t>
+        </is>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" t="n">
+        <v>2</v>
+      </c>
+      <c r="C37" t="n">
+        <v>38</v>
+      </c>
+      <c r="D37" t="n">
+        <v>2</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>2025-03-03 17:55:12</t>
+        </is>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2</v>
+      </c>
+      <c r="C38" t="n">
+        <v>39</v>
+      </c>
+      <c r="D38" t="n">
+        <v>3</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>2025-03-03 18:01:42</t>
+        </is>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2</v>
+      </c>
+      <c r="C39" t="n">
+        <v>40</v>
+      </c>
+      <c r="D39" t="n">
+        <v>3</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2025-03-03 18:05:52</t>
+        </is>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" t="n">
+        <v>2</v>
+      </c>
+      <c r="C40" t="n">
+        <v>41</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>2025-03-03 18:12:41</t>
+        </is>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" t="n">
+        <v>8</v>
+      </c>
+      <c r="C41" t="n">
+        <v>42</v>
+      </c>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>2025-03-03 18:19:56</t>
+        </is>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update order summary after successful item deletion
</commit_message>
<xml_diff>
--- a/Backup/Discounts.xlsx
+++ b/Backup/Discounts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1550,6 +1550,87 @@
         <v>0</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" t="n">
+        <v>2</v>
+      </c>
+      <c r="C42" t="n">
+        <v>43</v>
+      </c>
+      <c r="D42" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>2025-03-03 18:27:18</t>
+        </is>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42</v>
+      </c>
+      <c r="B43" t="n">
+        <v>2</v>
+      </c>
+      <c r="C43" t="n">
+        <v>44</v>
+      </c>
+      <c r="D43" t="n">
+        <v>12</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>2025-03-03 18:29:00</t>
+        </is>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43</v>
+      </c>
+      <c r="B44" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" t="n">
+        <v>45</v>
+      </c>
+      <c r="D44" t="n">
+        <v>23</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>2025-03-03 18:31:04</t>
+        </is>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix quantity and discount value handling in UI; ensure integer values are set
</commit_message>
<xml_diff>
--- a/Backup/Discounts.xlsx
+++ b/Backup/Discounts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1631,6 +1631,31 @@
         <v>0</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="n">
+        <v>46</v>
+      </c>
+      <c r="D45" t="n">
+        <v>18</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>2025-03-03 19:39:50</t>
+        </is>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor order update functionality: add order_info parameter and enhance UI for order management
</commit_message>
<xml_diff>
--- a/Backup/Discounts.xlsx
+++ b/Backup/Discounts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1656,6 +1656,33 @@
         <v>0</v>
       </c>
     </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="n">
+        <v>2</v>
+      </c>
+      <c r="C46" t="n">
+        <v>47</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>2025-03-04 07:04:08</t>
+        </is>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance shopkeeper management: add brand field to shopkeeper queries; implement product fetching by brand and add shopkeeper payment details retrieval
</commit_message>
<xml_diff>
--- a/Backup/Discounts.xlsx
+++ b/Backup/Discounts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -913,7 +913,7 @@
         <v>19</v>
       </c>
       <c r="D18" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -1237,7 +1237,7 @@
         <v>31</v>
       </c>
       <c r="D30" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1264,7 +1264,7 @@
         <v>32</v>
       </c>
       <c r="D31" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1680,6 +1680,33 @@
         </is>
       </c>
       <c r="G46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="n">
+        <v>7</v>
+      </c>
+      <c r="C47" t="n">
+        <v>48</v>
+      </c>
+      <c r="D47" t="n">
+        <v>4</v>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>2025-03-16 19:02:52</t>
+        </is>
+      </c>
+      <c r="G47" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance database management: update backup files for Payments, Orders, Discounts, and Shopkeepers; add new SQL triggers for payment and order updates
</commit_message>
<xml_diff>
--- a/Backup/Discounts.xlsx
+++ b/Backup/Discounts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,16 +472,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="n">
-        <v>54</v>
+        <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -490,7 +490,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-03-22 16:41:32</t>
+          <t>2025-03-23 21:55:01</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -499,16 +499,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -517,145 +517,10 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-03-22 16:58:33</t>
+          <t>2025-03-23 21:59:22</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>54</v>
-      </c>
-      <c r="B4" t="n">
-        <v>18</v>
-      </c>
-      <c r="C4" t="n">
-        <v>56</v>
-      </c>
-      <c r="D4" t="n">
-        <v>10</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>System</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>2025-03-22 17:08:42</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>55</v>
-      </c>
-      <c r="B5" t="n">
-        <v>17</v>
-      </c>
-      <c r="C5" t="n">
-        <v>57</v>
-      </c>
-      <c r="D5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>System</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>2025-03-22 17:24:12</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>56</v>
-      </c>
-      <c r="B6" t="n">
-        <v>19</v>
-      </c>
-      <c r="C6" t="n">
-        <v>58</v>
-      </c>
-      <c r="D6" t="n">
-        <v>5</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>System</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>2025-03-22 19:11:13</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>57</v>
-      </c>
-      <c r="B7" t="n">
-        <v>18</v>
-      </c>
-      <c r="C7" t="n">
-        <v>59</v>
-      </c>
-      <c r="D7" t="n">
-        <v>6</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>System</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>2025-03-22 19:16:46</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>58</v>
-      </c>
-      <c r="B8" t="n">
-        <v>18</v>
-      </c>
-      <c r="C8" t="n">
-        <v>60</v>
-      </c>
-      <c r="D8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>System</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2025-03-22 19:21:23</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance database management: update backup files for Khata, Orders, Payments, Discounts, and Order_Items; modify SQL queries to include Khata value and improve UI components
</commit_message>
<xml_diff>
--- a/Backup/Discounts.xlsx
+++ b/Backup/Discounts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,87 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>17</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-03-27 08:22:27</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>17</v>
+      </c>
+      <c r="C5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" t="n">
+        <v>15</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-03-27 15:28:01</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="n">
+        <v>18</v>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-03-27 17:20:34</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance database management: update backup files for Discounts, Khata, Order_Items, and Orders; add new SQL triggers for payment handling after order operations; adjust payments table UI for better column resizing
</commit_message>
<xml_diff>
--- a/Backup/Discounts.xlsx
+++ b/Backup/Discounts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,6 +605,60 @@
         <v>0</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>19</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-03-27 17:47:33</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="n">
+        <v>18</v>
+      </c>
+      <c r="C8" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-03-27 17:50:33</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance database management: update backup files for Khata, Orders, Payments, Discounts, and Order_Items; add SQL trigger for updating total sales on order updates; improve calculated sales and collections queries for salesmen
</commit_message>
<xml_diff>
--- a/Backup/Discounts.xlsx
+++ b/Backup/Discounts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -659,6 +659,222 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="n">
+        <v>20</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-03-28 18:18:25</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="n">
+        <v>20</v>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-03-28 18:41:45</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>16</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-03-28 19:07:07</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="n">
+        <v>16</v>
+      </c>
+      <c r="C12" t="n">
+        <v>11</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-03-28 19:17:33</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" t="n">
+        <v>16</v>
+      </c>
+      <c r="C13" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-03-28 19:18:43</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" t="n">
+        <v>16</v>
+      </c>
+      <c r="C14" t="n">
+        <v>13</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-03-28 19:19:42</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" t="n">
+        <v>16</v>
+      </c>
+      <c r="C15" t="n">
+        <v>14</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-03-28 19:21:47</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" t="n">
+        <v>16</v>
+      </c>
+      <c r="C16" t="n">
+        <v>15</v>
+      </c>
+      <c r="D16" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-03-28 19:22:09</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>